<commit_message>
Added resources_injector CLI tool
</commit_message>
<xml_diff>
--- a/tests/test_data/notice_transformer/mapping_suite_processor_repository/test_package_fake/transformation/conceptual_mappings.xlsx
+++ b/tests/test_data/notice_transformer/mapping_suite_processor_repository/test_package_fake/transformation/conceptual_mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -4201,7 +4201,7 @@
     <t xml:space="preserve">File name</t>
   </si>
   <si>
-    <t xml:space="preserve">countries.json</t>
+    <t xml:space="preserve">country.json</t>
   </si>
   <si>
     <t xml:space="preserve">nuts.json</t>
@@ -4981,11 +4981,11 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.67"/>
@@ -5103,8 +5103,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5123,7 +5123,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5148,8 +5148,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5168,7 +5168,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5193,8 +5193,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5213,7 +5213,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5238,8 +5238,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5258,7 +5258,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5283,8 +5283,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5303,7 +5303,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5328,8 +5328,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5348,15 +5348,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5377,7 +5377,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.22"/>
@@ -5386,7 +5386,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="26.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14281,8 +14281,8 @@
     <hyperlink ref="F126" r:id="rId14" display="VALUES/VAL_ESTIMATED_TOTAL/@CURRENCY"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14298,11 +14298,11 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.22"/>
   </cols>
@@ -14324,8 +14324,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14344,7 +14344,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.78"/>
@@ -14436,8 +14436,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14456,7 +14456,7 @@
       <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.66"/>
@@ -14598,8 +14598,8 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14618,7 +14618,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -14667,8 +14667,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14687,7 +14687,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -14728,8 +14728,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14748,7 +14748,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -14773,8 +14773,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14793,7 +14793,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -14818,8 +14818,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Updated CLI tests + docs
</commit_message>
<xml_diff>
--- a/tests/test_data/notice_transformer/mapping_suite_processor_repository/test_package_fake/transformation/conceptual_mappings.xlsx
+++ b/tests/test_data/notice_transformer/mapping_suite_processor_repository/test_package_fake/transformation/conceptual_mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -384,7 +384,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="720">
   <si>
     <t xml:space="preserve">Field</t>
   </si>
@@ -4223,34 +4223,25 @@
     <t xml:space="preserve">The first file listed should always be the main file (i.e. the "entry point" specific to a form)</t>
   </si>
   <si>
-    <t xml:space="preserve">contracting_authority.rml.ttl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">section 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">object.rml.ttl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">section 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procedure.rml.ttl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">section 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">award_of_contract.rml.ttl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">section 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">complementary_information.rml.ttl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">section 6</t>
+    <t xml:space="preserve">s1_contracting_authority.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s2_object.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s4_procedure.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s5_award_of_contract.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s6_complementary_information.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annex_d1.rml.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">result_notice.rml.ttl</t>
   </si>
   <si>
     <t xml:space="preserve">Property path</t>
@@ -5066,11 +5057,11 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.67"/>
@@ -5209,10 +5200,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5220,16 +5211,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="69" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -5254,10 +5245,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5265,16 +5256,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="69" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -5299,10 +5290,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5310,16 +5301,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="69" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -5344,10 +5335,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5355,16 +5346,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="69" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -5389,10 +5380,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5400,16 +5391,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="69" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -5434,10 +5425,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -5445,16 +5436,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="69" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>
@@ -5479,10 +5470,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -5508,10 +5499,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.22"/>
@@ -14433,10 +14424,10 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.22"/>
   </cols>
@@ -14472,13 +14463,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.25"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="54" t="s">
@@ -14500,40 +14494,35 @@
       <c r="A3" s="55" t="s">
         <v>677</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>678</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="55" t="s">
-        <v>679</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="55" t="s">
-        <v>681</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="55" t="s">
-        <v>683</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="55" t="s">
-        <v>685</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>686</v>
+        <v>681</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="55" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="55" t="s">
+        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -14555,10 +14544,10 @@
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.78"/>
@@ -14566,62 +14555,62 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="56" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="57" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="58" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="59" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="59" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="60" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11"/>
       <c r="B11" s="61" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="62" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="63" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="64" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14630,7 +14619,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="59" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="B16" s="33"/>
     </row>
@@ -14642,10 +14631,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="59" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
   </sheetData>
@@ -14667,10 +14656,10 @@
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.66"/>
@@ -14781,25 +14770,25 @@
         <v>65</v>
       </c>
       <c r="D5" s="66" t="s">
+        <v>700</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>701</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>702</v>
+      </c>
+      <c r="G5" s="67" t="s">
         <v>703</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="H5" s="68" t="s">
         <v>704</v>
       </c>
-      <c r="F5" s="67" t="s">
+      <c r="I5" s="66" t="s">
         <v>705</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="J5" s="67" t="s">
         <v>706</v>
-      </c>
-      <c r="H5" s="68" t="s">
-        <v>707</v>
-      </c>
-      <c r="I5" s="66" t="s">
-        <v>708</v>
-      </c>
-      <c r="J5" s="67" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14829,10 +14818,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
@@ -14840,40 +14829,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="69" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
   </sheetData>
@@ -14898,10 +14887,10 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -14909,32 +14898,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="69" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
   </sheetData>
@@ -14959,10 +14948,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
@@ -14970,16 +14959,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="69" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>